<commit_message>
test data commit 20200419
</commit_message>
<xml_diff>
--- a/日本語勉強システム/基本設計/domain.xlsx
+++ b/日本語勉強システム/基本設計/domain.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InnoX01\Desktop\日本語勉強システム設計\基本設計\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\study\language-study\日本語勉強システム\基本設計\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3ED260C-15E0-4F58-9458-A5956BBAB1C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B9668F-E3FC-4199-8848-55C93111F017}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0E10E1FD-25CA-46BE-A8B4-F68658EB13CC}"/>
+    <workbookView xWindow="9876" yWindow="5508" windowWidth="12252" windowHeight="7020" xr2:uid="{0E10E1FD-25CA-46BE-A8B4-F68658EB13CC}"/>
   </bookViews>
   <sheets>
     <sheet name="书本domain" sheetId="8" r:id="rId1"/>
@@ -2997,16 +2997,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
@@ -3015,10 +3015,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
@@ -3030,7 +3027,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
@@ -17102,168 +17102,168 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A67EA24-652D-43A7-9E59-5732E631A81D}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="17" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15" t="s">
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15" t="s">
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15" t="s">
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15" t="s">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15" t="s">
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15" t="s">
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15" t="s">
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15" t="s">
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15" t="s">
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15" t="s">
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="12" t="s">
         <v>142</v>
       </c>
@@ -17272,22 +17272,7 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:O5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
@@ -17300,7 +17285,22 @@
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17312,9 +17312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6065C6C-A809-438F-B81D-C63726058870}">
   <dimension ref="A2:R36"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -17353,161 +17351,161 @@
       <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15" t="s">
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15" t="s">
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15" t="s">
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="17" t="s">
         <v>26</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15" t="s">
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15" t="s">
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15" t="s">
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15" t="s">
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15" t="s">
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15" t="s">
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15" t="s">
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15" t="s">
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15" t="s">
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15" t="s">
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15" t="s">
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15" t="s">
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15" t="s">
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
       <c r="M35" s="12" t="s">
         <v>121</v>
       </c>
@@ -17515,26 +17513,26 @@
       <c r="O35" s="5"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15" t="s">
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15" t="s">
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15" t="s">
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
       <c r="M36" s="5" t="s">
         <v>122</v>
       </c>
@@ -17544,23 +17542,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:L31"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="G36:I36"/>
@@ -17577,6 +17558,23 @@
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="J30:L30"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G35:I35"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17589,9 +17587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D6365C-5EAB-4814-8455-42161173F591}">
   <dimension ref="A3:P54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -17636,124 +17632,124 @@
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="22" t="s">
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="18" t="s">
         <v>22</v>
       </c>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
       <c r="G39" s="20"/>
-      <c r="H39" s="15" t="s">
+      <c r="H39" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15" t="s">
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="26" t="s">
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="21" t="s">
         <v>162</v>
       </c>
       <c r="O39" s="19"/>
       <c r="P39" s="20"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="22" t="s">
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="18" t="s">
         <v>51</v>
       </c>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="20"/>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15" t="s">
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="23" t="s">
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O40" s="24"/>
-      <c r="P40" s="25"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="24"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="22" t="s">
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="18" t="s">
         <v>101</v>
       </c>
       <c r="E41" s="19"/>
       <c r="F41" s="19"/>
       <c r="G41" s="20"/>
-      <c r="H41" s="15" t="s">
+      <c r="H41" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15" t="s">
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="22" t="s">
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="18" t="s">
         <v>52</v>
       </c>
       <c r="O41" s="19"/>
       <c r="P41" s="20"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="22" t="s">
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="18" t="s">
         <v>50</v>
       </c>
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
       <c r="G42" s="20"/>
-      <c r="H42" s="15" t="s">
+      <c r="H42" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15" t="s">
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="22" t="s">
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="18" t="s">
         <v>59</v>
       </c>
       <c r="O42" s="19"/>
       <c r="P42" s="20"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="22" t="s">
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="18" t="s">
         <v>153</v>
       </c>
       <c r="E43" s="19"/>
@@ -17764,22 +17760,22 @@
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="22" t="s">
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="18" t="s">
         <v>156</v>
       </c>
       <c r="O43" s="19"/>
       <c r="P43" s="20"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="26" t="s">
         <v>148</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="18" t="s">
         <v>159</v>
       </c>
       <c r="E44" s="19"/>
@@ -17790,22 +17786,22 @@
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="18" t="s">
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="25" t="s">
         <v>170</v>
       </c>
       <c r="O44" s="19"/>
       <c r="P44" s="20"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="26" t="s">
         <v>164</v>
       </c>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="18" t="s">
         <v>167</v>
       </c>
       <c r="E45" s="19"/>
@@ -17816,22 +17812,22 @@
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="18" t="s">
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="25" t="s">
         <v>171</v>
       </c>
       <c r="O45" s="19"/>
       <c r="P45" s="20"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="22" t="s">
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="18" t="s">
         <v>154</v>
       </c>
       <c r="E46" s="19"/>
@@ -17842,22 +17838,22 @@
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="22" t="s">
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="18" t="s">
         <v>157</v>
       </c>
       <c r="O46" s="19"/>
       <c r="P46" s="20"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="26" t="s">
         <v>149</v>
       </c>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="18" t="s">
         <v>160</v>
       </c>
       <c r="E47" s="19"/>
@@ -17868,22 +17864,22 @@
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="18" t="s">
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="25" t="s">
         <v>172</v>
       </c>
       <c r="O47" s="19"/>
       <c r="P47" s="20"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="26" t="s">
         <v>165</v>
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="18" t="s">
         <v>168</v>
       </c>
       <c r="E48" s="19"/>
@@ -17894,95 +17890,95 @@
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="18" t="s">
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="25" t="s">
         <v>173</v>
       </c>
       <c r="O48" s="19"/>
       <c r="P48" s="20"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="23" t="s">
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="25"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="24"/>
       <c r="H49" s="5" t="s">
         <v>189</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="22" t="s">
+      <c r="K49" s="16"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="18" t="s">
         <v>158</v>
       </c>
       <c r="O49" s="19"/>
       <c r="P49" s="20"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A50" s="21" t="s">
+      <c r="A50" s="26" t="s">
         <v>129</v>
       </c>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
-      <c r="D50" s="23" t="s">
+      <c r="D50" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="25"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="24"/>
       <c r="H50" s="5" t="s">
         <v>189</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
-      <c r="K50" s="15"/>
-      <c r="L50" s="15"/>
-      <c r="M50" s="15"/>
-      <c r="N50" s="18" t="s">
+      <c r="K50" s="16"/>
+      <c r="L50" s="16"/>
+      <c r="M50" s="16"/>
+      <c r="N50" s="25" t="s">
         <v>174</v>
       </c>
       <c r="O50" s="19"/>
       <c r="P50" s="20"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A51" s="21" t="s">
+      <c r="A51" s="26" t="s">
         <v>166</v>
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
-      <c r="D51" s="23" t="s">
+      <c r="D51" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="25"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="24"/>
       <c r="H51" s="5" t="s">
         <v>189</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="18" t="s">
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="25" t="s">
         <v>175</v>
       </c>
       <c r="O51" s="19"/>
       <c r="P51" s="20"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="26" t="s">
         <v>127</v>
       </c>
       <c r="B52" s="17"/>
@@ -17993,44 +17989,44 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="11"/>
-      <c r="H52" s="15" t="s">
+      <c r="H52" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15" t="s">
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15" t="s">
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="22" t="s">
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="18" t="s">
         <v>102</v>
       </c>
       <c r="E53" s="19"/>
       <c r="F53" s="19"/>
       <c r="G53" s="20"/>
-      <c r="H53" s="15" t="s">
+      <c r="H53" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15" t="s">
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
       <c r="N53" s="13" t="s">
         <v>123</v>
       </c>
@@ -18038,27 +18034,27 @@
       <c r="P53" s="8"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="22" t="s">
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="18" t="s">
         <v>103</v>
       </c>
       <c r="E54" s="19"/>
       <c r="F54" s="19"/>
       <c r="G54" s="20"/>
-      <c r="H54" s="15" t="s">
+      <c r="H54" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15" t="s">
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
       <c r="N54" s="6" t="s">
         <v>124</v>
       </c>
@@ -18067,6 +18063,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="N48:P48"/>
+    <mergeCell ref="N50:P50"/>
+    <mergeCell ref="N51:P51"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="N49:P49"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="K54:M54"/>
+    <mergeCell ref="N46:P46"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="N45:P45"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="N40:P40"/>
+    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="N42:P42"/>
+    <mergeCell ref="N43:P43"/>
     <mergeCell ref="K52:M52"/>
     <mergeCell ref="K46:M46"/>
     <mergeCell ref="D39:G39"/>
@@ -18083,58 +18131,6 @@
     <mergeCell ref="K41:M41"/>
     <mergeCell ref="D40:G40"/>
     <mergeCell ref="H40:J40"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="N42:P42"/>
-    <mergeCell ref="N43:P43"/>
-    <mergeCell ref="N46:P46"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="H54:J54"/>
-    <mergeCell ref="K54:M54"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="N48:P48"/>
-    <mergeCell ref="N50:P50"/>
-    <mergeCell ref="N51:P51"/>
-    <mergeCell ref="N52:P52"/>
-    <mergeCell ref="N49:P49"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18173,53 +18169,53 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="22" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="18" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15" t="s">
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="22" t="s">
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="18" t="s">
         <v>41</v>
       </c>
       <c r="N28" s="19"/>
       <c r="O28" s="20"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="22" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="18" t="s">
         <v>91</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15" t="s">
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
       <c r="M29" s="27" t="s">
         <v>68</v>
       </c>
@@ -18227,61 +18223,61 @@
       <c r="O29" s="29"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="22" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="18" t="s">
         <v>93</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15" t="s">
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="22" t="s">
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="18" t="s">
         <v>69</v>
       </c>
       <c r="N30" s="19"/>
       <c r="O30" s="20"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="22" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="18" t="s">
         <v>95</v>
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
-      <c r="G31" s="15" t="s">
+      <c r="G31" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15" t="s">
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="22" t="s">
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="18" t="s">
         <v>96</v>
       </c>
       <c r="N31" s="19"/>
       <c r="O31" s="20"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="26" t="s">
         <v>179</v>
       </c>
       <c r="B32" s="17"/>
@@ -18291,43 +18287,43 @@
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
-      <c r="G32" s="15" t="s">
+      <c r="G32" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15" t="s">
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15" t="s">
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="22" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="18" t="s">
         <v>62</v>
       </c>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
-      <c r="G33" s="15" t="s">
+      <c r="G33" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15" t="s">
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
       <c r="M33" s="13" t="s">
         <v>70</v>
       </c>
@@ -18335,26 +18331,26 @@
       <c r="O33" s="8"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="22" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15" t="s">
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
       <c r="M34" s="6" t="s">
         <v>125</v>
       </c>
@@ -18363,16 +18359,14 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:L33"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="G32:I32"/>
     <mergeCell ref="J32:L32"/>
@@ -18387,14 +18381,16 @@
     <mergeCell ref="G31:I31"/>
     <mergeCell ref="J31:L31"/>
     <mergeCell ref="M31:O31"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="M29:O29"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18406,7 +18402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83672613-B5BF-48BC-98BB-0C71B0DC51F3}">
   <dimension ref="A2:O32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
@@ -18438,53 +18434,53 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="22" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="18" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15" t="s">
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="22" t="s">
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="18" t="s">
         <v>41</v>
       </c>
       <c r="N26" s="19"/>
       <c r="O26" s="20"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="22" t="s">
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="18" t="s">
         <v>71</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15" t="s">
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
       <c r="M27" s="27" t="s">
         <v>78</v>
       </c>
@@ -18492,61 +18488,61 @@
       <c r="O27" s="29"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="22" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="18" t="s">
         <v>72</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15" t="s">
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="22" t="s">
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="18" t="s">
         <v>79</v>
       </c>
       <c r="N28" s="19"/>
       <c r="O28" s="20"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="22" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="18" t="s">
         <v>105</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15" t="s">
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="22" t="s">
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="18" t="s">
         <v>109</v>
       </c>
       <c r="N29" s="19"/>
       <c r="O29" s="20"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="26" t="s">
         <v>180</v>
       </c>
       <c r="B30" s="17"/>
@@ -18556,43 +18552,43 @@
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15" t="s">
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15" t="s">
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="22" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="18" t="s">
         <v>73</v>
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
-      <c r="G31" s="15" t="s">
+      <c r="G31" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15" t="s">
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
       <c r="M31" s="13" t="s">
         <v>80</v>
       </c>
@@ -18600,26 +18596,26 @@
       <c r="O31" s="8"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="22" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="18" t="s">
         <v>74</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
-      <c r="G32" s="15" t="s">
+      <c r="G32" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15" t="s">
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
       <c r="M32" s="6" t="s">
         <v>126</v>
       </c>
@@ -18628,22 +18624,11 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:L31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="D32:F32"/>
     <mergeCell ref="G32:I32"/>
@@ -18655,11 +18640,22 @@
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="G30:I30"/>
     <mergeCell ref="J30:L30"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="M27:O27"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18671,8 +18667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D311425-F2F2-4AB0-8540-A5B72BA44F71}">
   <dimension ref="A2:P31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25:I25"/>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -18703,53 +18699,53 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="22" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="18" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15" t="s">
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="22" t="s">
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="18" t="s">
         <v>41</v>
       </c>
       <c r="N25" s="19"/>
       <c r="O25" s="20"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="22" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="18" t="s">
         <v>81</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15" t="s">
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
       <c r="M26" s="27" t="s">
         <v>88</v>
       </c>
@@ -18757,54 +18753,54 @@
       <c r="O26" s="29"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="22" t="s">
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="18" t="s">
         <v>82</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15" t="s">
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="22" t="s">
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="18" t="s">
         <v>89</v>
       </c>
       <c r="N27" s="19"/>
       <c r="O27" s="20"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="22" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="18" t="s">
         <v>112</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15" t="s">
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="22" t="s">
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="18" t="s">
         <v>116</v>
       </c>
       <c r="N28" s="19"/>
@@ -18821,43 +18817,43 @@
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15" t="s">
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15" t="s">
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="22" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="18" t="s">
         <v>83</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15" t="s">
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
       <c r="M30" s="6" t="s">
         <v>118</v>
       </c>
@@ -18866,26 +18862,26 @@
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="22" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="18" t="s">
         <v>84</v>
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
-      <c r="G31" s="15" t="s">
+      <c r="G31" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15" t="s">
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
       <c r="M31" s="6" t="s">
         <v>120</v>
       </c>
@@ -18895,22 +18891,11 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:L30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="D31:F31"/>
     <mergeCell ref="G31:I31"/>
@@ -18922,11 +18907,22 @@
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="G29:I29"/>
     <mergeCell ref="J29:L29"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="M26:O26"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>